<commit_message>
Fixed "could not find the object '.Dual'"-error for real.
</commit_message>
<xml_diff>
--- a/ExcelDBviaEntityFramework/Excel files/Signups_v2.xlsx
+++ b/ExcelDBviaEntityFramework/Excel files/Signups_v2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emiel.Nijhuis\source\repos\misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emiel.Nijhuis\source\repos\misc\ExcelDBviaEntityFramework\ExcelDBviaEntityFramework\Excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14C67D6-3F5A-47AB-9AC1-CB35AF94F237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B9098B-3BA8-44F3-A5E3-6D5FC14A65A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-1410" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -404,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="ShSignups"/>
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">

</xml_diff>

<commit_message>
Implemented logging of upserts
</commit_message>
<xml_diff>
--- a/ExcelDBviaEntityFramework/Excel files/Signups_v2.xlsx
+++ b/ExcelDBviaEntityFramework/Excel files/Signups_v2.xlsx
@@ -5,16 +5,20 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emiel.Nijhuis\source\repos\misc\ExcelDBviaEntityFramework\ExcelDBviaEntityFramework\Excel files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emiel.Nijhuis\source\repos\misc\ExcelDBviaEntityFramework\ExcelDBviaEntityFramework\bin\Debug\net8.0\Excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32226948-BC70-4E70-BCFC-CDC526D128F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAF85C4-0A85-418D-A426-2FE4F883B40B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57270" yWindow="1920" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Signups" sheetId="1" r:id="rId1"/>
+    <sheet name="Log" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Log!$A$1:$D$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +38,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+  <si>
+    <t>Deleted_ý</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
   <si>
     <t>Name</t>
   </si>
@@ -51,6 +61,9 @@
     <t>555-5551</t>
   </si>
   <si>
+    <t>x</t>
+  </si>
+  <si>
     <t>Ryan</t>
   </si>
   <si>
@@ -63,19 +76,46 @@
     <t>555-5553</t>
   </si>
   <si>
-    <t>Deleted_ý</t>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>x</t>
+    <t>xb</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>Signup id</t>
+  </si>
+  <si>
+    <t>Entry</t>
+  </si>
+  <si>
+    <t>6c02363c</t>
+  </si>
+  <si>
+    <t>Added signup: Name: tertert, Phone: 444-5555, Party Size: 5</t>
+  </si>
+  <si>
+    <t>c7a94c78</t>
+  </si>
+  <si>
+    <t>xbb</t>
+  </si>
+  <si>
+    <t>Added signup: Name: sd, Phone: asd, Party Size: 3</t>
+  </si>
+  <si>
+    <t>dc7470e2</t>
+  </si>
+  <si>
+    <t>Updated signup: Name: [unchanged], Phone: 5345, Party Size: 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d/mm/yyyy\ h:mm:ss;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,11 +159,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,7 +452,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,19 +466,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -445,13 +489,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -459,16 +503,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -479,10 +523,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -492,4 +536,80 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1747548-7ABD-4ACC-9E21-FDDFD78FD57B}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="78.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="5">
+        <v>45887.650567129604</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="5">
+        <v>45887.677777777797</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="4">
+        <v>45887.681678240697</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Made UIActions injectable and populated Excel file
</commit_message>
<xml_diff>
--- a/ExcelDBviaEntityFramework/Excel files/Signups_v2.xlsx
+++ b/ExcelDBviaEntityFramework/Excel files/Signups_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emiel.Nijhuis\source\repos\misc\ExcelDBviaEntityFramework\ExcelDBviaEntityFramework\Excel files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emiel.Nijhuis\source\repos\misc\ExcelDBviaEntityFramework\ExcelDBviaEntityFramework\bin\Debug\net8.0\Excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F1E903-5313-4752-910E-13E8EE446AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF39B7D-9571-41E4-8AB5-58169290056C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57270" yWindow="1920" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="54864" yWindow="-7176" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Signups" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>Deleted_ý</t>
   </si>
@@ -55,15 +55,57 @@
     <t>Party size</t>
   </si>
   <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>Signup id</t>
+  </si>
+  <si>
+    <t>Entry</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>Brice</t>
   </si>
   <si>
     <t>555-5551</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>ea3bdcd5</t>
+  </si>
+  <si>
+    <t>Added signup: Name: Brice, Phone: 555-5551, Party Size: 3</t>
+  </si>
+  <si>
+    <t>John.Doe</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>Ryan</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>33427300</t>
+  </si>
+  <si>
+    <t>Added signup: Name: Ryan, Phone: 555-5559, Party Size: 4</t>
+  </si>
+  <si>
     <t>555-5552</t>
   </si>
   <si>
@@ -73,28 +115,16 @@
     <t>555-5553</t>
   </si>
   <si>
-    <t>Timestamp</t>
-  </si>
-  <si>
-    <t>Signup id</t>
-  </si>
-  <si>
-    <t>Entry</t>
-  </si>
-  <si>
-    <t>dc7470e2</t>
-  </si>
-  <si>
-    <t>Updated signup: Name: [unchanged], Phone: 5345, Party Size: 4</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>John.Doe</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>8187ebee</t>
+  </si>
+  <si>
+    <t>Updated signup: Name: [unchanged], Phone: 555-5552, Party Size: [unchanged]</t>
+  </si>
+  <si>
+    <t>25548527</t>
+  </si>
+  <si>
+    <t>Added signup: Name: David, Phone: 555-5553, Party Size: 2</t>
   </si>
 </sst>
 </file>
@@ -102,7 +132,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d/mm/yyyy\ h:mm:ss;@"/>
+    <numFmt numFmtId="164" formatCode="d/mm/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -440,16 +470,16 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,55 +496,55 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="b">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="b">
-        <v>0</v>
-      </c>
-      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3">
-        <v>3</v>
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -525,51 +555,102 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1747548-7ABD-4ACC-9E21-FDDFD78FD57B}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
     <col min="3" max="3" width="19" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="78.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="78.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="4">
-        <v>45887.681678240697</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1</v>
+        <v>45888.5568055556</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="4">
+        <v>45888.559282407397</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4">
+        <v>45888.480891203704</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="4">
+        <v>45888.482013888897</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Restored soft deletes because of issues with ClosedXML
</commit_message>
<xml_diff>
--- a/ExcelDBviaEntityFramework/Excel files/Signups_v2.xlsx
+++ b/ExcelDBviaEntityFramework/Excel files/Signups_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emiel.Nijhuis\source\repos\misc\ExcelDBviaEntityFramework\ExcelDBviaEntityFramework\bin\Debug\net8.0\Excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF39B7D-9571-41E4-8AB5-58169290056C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF0BB1B-FEB1-4CE1-9A88-35B5881D8CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="54864" yWindow="-7176" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Log" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Log!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Log!$B$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,10 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
-  <si>
-    <t>Deleted_ý</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Id</t>
   </si>
@@ -125,6 +122,9 @@
   </si>
   <si>
     <t>Added signup: Name: David, Phone: 555-5553, Party Size: 2</t>
+  </si>
+  <si>
+    <t>Deleted</t>
   </si>
 </sst>
 </file>
@@ -466,13 +466,11 @@
   <sheetPr codeName="ShSignups"/>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
     <col min="2" max="2" width="11" style="3" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5546875" customWidth="1"/>
@@ -481,70 +479,70 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -555,106 +553,122 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1747548-7ABD-4ACC-9E21-FDDFD78FD57B}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
-    <col min="3" max="3" width="19" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="78.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="19" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="78.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4">
+        <v>45888.5568055556</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4">
+        <v>45888.559282407397</v>
+      </c>
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="4">
-        <v>45888.5568055556</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D4" s="4">
+        <v>45888.480891203697</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4">
-        <v>45888.559282407397</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="F4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="4">
-        <v>45888.480891203704</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4">
+        <v>45888.482013888897</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="4">
-        <v>45888.482013888897</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="B1:F1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Removed optional cascade delete.
</commit_message>
<xml_diff>
--- a/ExcelDBviaEntityFramework/Excel files/Signups_v2.xlsx
+++ b/ExcelDBviaEntityFramework/Excel files/Signups_v2.xlsx
@@ -5,19 +5,20 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emiel.Nijhuis\source\repos\misc\ExcelDBviaEntityFramework\ExcelDBviaEntityFramework\bin\Debug\net8.0\Excel files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emiel.Nijhuis\source\repos\misc\ExcelDBviaEntityFramework\ExcelDBviaEntityFramework\Excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF0BB1B-FEB1-4CE1-9A88-35B5881D8CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F02FBBC-5759-4E13-BBAD-4C139DC7C24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54864" yWindow="-7176" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="53652" yWindow="-11424" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Signups" sheetId="1" r:id="rId1"/>
     <sheet name="Log" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Log!$B$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Log!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Signups!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -470,7 +471,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="11" style="3" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5546875" customWidth="1"/>
@@ -478,7 +479,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -546,6 +547,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -559,16 +561,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" customWidth="1"/>
     <col min="3" max="3" width="18.5546875" customWidth="1"/>
-    <col min="4" max="4" width="19" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" style="4" customWidth="1"/>
     <col min="5" max="5" width="12.109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="78.33203125" customWidth="1"/>
+    <col min="6" max="6" width="108.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -648,7 +650,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
@@ -668,7 +670,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:F1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:F1" xr:uid="{A1747548-7ABD-4ACC-9E21-FDDFD78FD57B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented first service test in SignupServiceTests
</commit_message>
<xml_diff>
--- a/ExcelDBviaEntityFramework/Excel files/Signups_v2.xlsx
+++ b/ExcelDBviaEntityFramework/Excel files/Signups_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emiel.Nijhuis\source\repos\misc\ExcelDBviaEntityFramework\ExcelDBviaEntityFramework\Excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F02FBBC-5759-4E13-BBAD-4C139DC7C24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD3627F-A842-4202-9548-42339AF19BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53652" yWindow="-11424" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="53880" yWindow="-1410" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Signups" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Id</t>
   </si>
@@ -98,9 +98,6 @@
     <t>4</t>
   </si>
   <si>
-    <t>33427300</t>
-  </si>
-  <si>
     <t>Added signup: Name: Ryan, Phone: 555-5559, Party Size: 4</t>
   </si>
   <si>
@@ -119,13 +116,19 @@
     <t>Updated signup: Name: [unchanged], Phone: 555-5552, Party Size: [unchanged]</t>
   </si>
   <si>
-    <t>25548527</t>
-  </si>
-  <si>
     <t>Added signup: Name: David, Phone: 555-5553, Party Size: 2</t>
   </si>
   <si>
     <t>Deleted</t>
+  </si>
+  <si>
+    <t>Michael.Smith</t>
+  </si>
+  <si>
+    <t>334273x0</t>
+  </si>
+  <si>
+    <t>25y48527</t>
   </si>
 </sst>
 </file>
@@ -469,18 +472,18 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="11" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -495,7 +498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -512,7 +515,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -523,13 +526,13 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -537,10 +540,10 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
         <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -559,19 +562,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="108.21875" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="108.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -589,7 +592,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -609,64 +612,64 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D3" s="4">
-        <v>45888.559282407397</v>
+        <v>45888.64261574074</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D4" s="4">
-        <v>45888.480891203697</v>
+        <v>45889.43922453704</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="4">
-        <v>45888.482013888897</v>
+        <v>45889.48201388889</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>